<commit_message>
--IBBS Web App Metrics: Version 1.2--
This project was synced upstream with version 1.2 (git tag: web_app_metrics_v1.2) of the web app metrics project (git@picgitlab.nmfs.local:centralized-data-tools/web-app-metrics.git)

	Docker Files:
		python scripts:
			docker/src/py_scripts/lib/custom_functions.py - was updated to capture case-insensitive content-length and Content-Length values from the performance logs

	performance metrics/ibbs-web-app-metrics-combined.xlsx was updated to remove the existing detailed data

	Documentation:
		README.md - was updated to increment the version number
</commit_message>
<xml_diff>
--- a/performance metrics/ibbs-web-app-metrics-combined.xlsx
+++ b/performance metrics/ibbs-web-app-metrics-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\ibbs-web-app-metrics\performance metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F0152-A6CA-4B52-A190-90EFC8B35222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9ED427-2BBD-495D-AEE8-871570BDCEF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ibbs-web-app-metrics" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="33">
   <si>
     <t>Date/Time</t>
   </si>
@@ -119,22 +119,10 @@
     <t>Screenshot File</t>
   </si>
   <si>
-    <t>IBBS APEX app</t>
-  </si>
-  <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>remote</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
     <t>Page Load</t>
-  </si>
-  <si>
-    <t>Login.png</t>
   </si>
   <si>
     <t>Full Sampling Plan Report</t>
@@ -143,31 +131,16 @@
     <t>Login/Page Load</t>
   </si>
   <si>
-    <t>Full Sampling Plan Report.png</t>
-  </si>
-  <si>
     <t>Page Reload/Filter Report</t>
-  </si>
-  <si>
-    <t>Full Sampling Plan Report filter.png</t>
   </si>
   <si>
     <t>View Specimens</t>
   </si>
   <si>
-    <t>View Specimens.png</t>
-  </si>
-  <si>
     <t>View/Edit Specimen</t>
   </si>
   <si>
-    <t>View Edit Specimen.png</t>
-  </si>
-  <si>
     <t>Form submission</t>
-  </si>
-  <si>
-    <t>View Edit Specimen post specimen record insert.png</t>
   </si>
   <si>
     <t>Ratio Remote/Local</t>
@@ -884,21 +857,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -915,6 +873,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1274,9 +1247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J636"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:F7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,643 +1296,67 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="17">
-        <v>45512.556319444448</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2">
-        <v>25</v>
-      </c>
-      <c r="H2" s="14">
-        <v>691.42</v>
-      </c>
-      <c r="I2">
-        <v>2.6920000000000002</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="17">
-        <v>45512.556354166663</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3">
-        <v>46</v>
-      </c>
-      <c r="H3" s="14">
-        <v>1115.9000000000001</v>
-      </c>
-      <c r="I3">
-        <v>2.78</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="17">
-        <v>45512.556388888886</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4">
-        <v>50</v>
-      </c>
-      <c r="H4" s="14">
-        <v>1121.7</v>
-      </c>
-      <c r="I4">
-        <v>2.2370000000000001</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="17">
-        <v>45512.556423611109</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5">
-        <v>45</v>
-      </c>
-      <c r="H5" s="14">
-        <v>1451.97</v>
-      </c>
-      <c r="I5">
-        <v>4.0449999999999999</v>
-      </c>
-      <c r="J5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="17">
-        <v>45512.556469907409</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>31</v>
-      </c>
-      <c r="H6" s="14">
-        <v>609.77</v>
-      </c>
-      <c r="I6">
-        <v>1.724</v>
-      </c>
-      <c r="J6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="17">
-        <v>45512.556539351855</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7">
-        <v>61</v>
-      </c>
-      <c r="H7" s="14">
-        <v>1369.75</v>
-      </c>
-      <c r="I7">
-        <v>8.2089999999999996</v>
-      </c>
-      <c r="J7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="17">
-        <v>45512.556990740741</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8">
-        <v>24</v>
-      </c>
-      <c r="H8" s="14">
-        <v>26.23</v>
-      </c>
-      <c r="I8">
-        <v>3.6869999999999998</v>
-      </c>
-      <c r="J8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="17">
-        <v>45512.557037037041</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9">
-        <v>41</v>
-      </c>
-      <c r="H9" s="14">
-        <v>1974.42</v>
-      </c>
-      <c r="I9">
-        <v>2.7130000000000001</v>
-      </c>
-      <c r="J9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="17">
-        <v>45512.557071759256</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10">
-        <v>41</v>
-      </c>
-      <c r="H10" s="14">
-        <v>3833.54</v>
-      </c>
-      <c r="I10">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="J10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="17">
-        <v>45512.55709490741</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11">
-        <v>34</v>
-      </c>
-      <c r="H11" s="14">
-        <v>3146.74</v>
-      </c>
-      <c r="I11">
-        <v>4.8339999999999996</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="17">
-        <v>45512.557152777779</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12">
-        <v>35</v>
-      </c>
-      <c r="H12" s="14">
-        <v>3142.13</v>
-      </c>
-      <c r="I12">
-        <v>1.6639999999999999</v>
-      </c>
-      <c r="J12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="17">
-        <v>45512.557222222225</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13">
-        <v>54</v>
-      </c>
-      <c r="H13" s="14">
-        <v>3854.18</v>
-      </c>
-      <c r="I13">
-        <v>4.915</v>
-      </c>
-      <c r="J13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="17">
-        <v>45512.559178240743</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14">
-        <v>24</v>
-      </c>
-      <c r="H14" s="14">
-        <v>690.32</v>
-      </c>
-      <c r="I14">
-        <v>3.3679999999999999</v>
-      </c>
-      <c r="J14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="17">
-        <v>45512.559224537035</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15">
-        <v>49</v>
-      </c>
-      <c r="H15" s="14">
-        <v>1119.9100000000001</v>
-      </c>
-      <c r="I15">
-        <v>4.3719999999999999</v>
-      </c>
-      <c r="J15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="17">
-        <v>45512.559270833335</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16">
-        <v>48</v>
-      </c>
-      <c r="H16" s="14">
-        <v>1118.81</v>
-      </c>
-      <c r="I16">
-        <v>3.52</v>
-      </c>
-      <c r="J16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="17">
-        <v>45512.559317129628</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17">
-        <v>43</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1214.9000000000001</v>
-      </c>
-      <c r="I17">
-        <v>7.29</v>
-      </c>
-      <c r="J17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="17">
-        <v>45512.55940972222</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18">
-        <v>33</v>
-      </c>
-      <c r="H18" s="14">
-        <v>846.83</v>
-      </c>
-      <c r="I18">
-        <v>3.0129999999999999</v>
-      </c>
-      <c r="J18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="17">
-        <v>45512.559490740743</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19">
-        <v>61</v>
-      </c>
-      <c r="H19" s="14">
-        <v>1369.77</v>
-      </c>
-      <c r="I19">
-        <v>4.74</v>
-      </c>
-      <c r="J19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D20" s="15"/>
       <c r="E20"/>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D21" s="15"/>
       <c r="E21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D22" s="15"/>
       <c r="E22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D23" s="15"/>
       <c r="E23"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D24" s="15"/>
       <c r="E24"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D25" s="15"/>
       <c r="E25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D26" s="15"/>
       <c r="E26"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D27" s="15"/>
       <c r="E27"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D28" s="15"/>
       <c r="E28"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D29" s="15"/>
       <c r="E29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D30" s="15"/>
       <c r="E30"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D31" s="15"/>
       <c r="E31"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D32" s="15"/>
       <c r="E32"/>
       <c r="H32"/>
@@ -4994,8 +4391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="AO13" sqref="AO13"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="AT3" sqref="AT3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,72 +4405,72 @@
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="44" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="42" t="s">
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="42"/>
-      <c r="Q1" s="42"/>
-      <c r="R1" s="42"/>
-      <c r="S1" s="42"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="50" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="52"/>
-      <c r="Z1" s="50" t="s">
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="52"/>
-      <c r="AE1" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="49"/>
-      <c r="AO1" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="49"/>
-      <c r="AT1" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="49"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="43"/>
+      <c r="AG1" s="43"/>
+      <c r="AH1" s="43"/>
+      <c r="AI1" s="44"/>
+      <c r="AJ1" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="43"/>
+      <c r="AM1" s="43"/>
+      <c r="AN1" s="44"/>
+      <c r="AO1" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="43"/>
+      <c r="AQ1" s="43"/>
+      <c r="AR1" s="43"/>
+      <c r="AS1" s="44"/>
+      <c r="AT1" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="AU1" s="43"/>
+      <c r="AV1" s="43"/>
+      <c r="AW1" s="43"/>
+      <c r="AX1" s="44"/>
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -5229,30 +4626,30 @@
     </row>
     <row r="3" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" s="18" cm="1">
         <f t="array" ref="C3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="19" cm="1">
         <f t="array" ref="D3">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.6869999999999998</v>
+        <v>0</v>
       </c>
       <c r="E3" s="19" cm="1">
         <f t="array" ref="E3">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.6869999999999998</v>
-      </c>
-      <c r="F3" s="19" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="19" t="e" cm="1">
         <f t="array" ref="F3">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.6869999999999998</v>
-      </c>
-      <c r="G3" s="19" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G3" s="19" t="e" cm="1">
         <f t="array" ref="G3">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.6869999999999998</v>
+        <v>#NUM!</v>
       </c>
       <c r="H3" s="20" t="e" cm="1">
         <f t="array" ref="H3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5260,27 +4657,27 @@
       </c>
       <c r="I3" s="19" cm="1">
         <f t="array" ref="I3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" s="19" cm="1">
         <f t="array" ref="J3">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.6920000000000002</v>
+        <v>0</v>
       </c>
       <c r="K3" s="19" cm="1">
         <f t="array" ref="K3">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.3679999999999999</v>
-      </c>
-      <c r="L3" s="19" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="19" t="e" cm="1">
         <f t="array" ref="L3">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.0300000000000002</v>
-      </c>
-      <c r="M3" s="19" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M3" s="19" t="e" cm="1">
         <f t="array" ref="M3">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.0300000000000002</v>
-      </c>
-      <c r="N3" s="20" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N3" s="20" t="e" cm="1">
         <f t="array" ref="N3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>0.47800418408210477</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O3" s="19" cm="1">
         <f t="array" ref="O3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5306,21 +4703,21 @@
         <f t="array" ref="T3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U3" s="39">
+      <c r="U3" s="39" t="e">
         <f>J3/D3</f>
-        <v>0.73013289937618664</v>
-      </c>
-      <c r="V3" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V3" s="8" t="e">
         <f>K3/E3</f>
-        <v>0.91347979387035527</v>
-      </c>
-      <c r="W3" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W3" s="8" t="e">
         <f>L3/F3</f>
-        <v>0.82180634662327101</v>
-      </c>
-      <c r="X3" s="8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X3" s="8" t="e">
         <f>M3/G3</f>
-        <v>0.82180634662327101</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y3" s="9" t="e">
         <f>N3/H3</f>
@@ -5328,31 +4725,31 @@
       </c>
       <c r="Z3" s="10">
         <f>J3-D3</f>
-        <v>-0.99499999999999966</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="11">
         <f>K3-E3</f>
-        <v>-0.31899999999999995</v>
-      </c>
-      <c r="AB3" s="11">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="11" t="e">
         <f>L3-F3</f>
-        <v>-0.65699999999999958</v>
-      </c>
-      <c r="AC3" s="11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC3" s="11" t="e">
         <f>M3-G3</f>
-        <v>-0.65699999999999958</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD3" s="12" t="e">
         <f>N3-H3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE3" s="10">
+      <c r="AE3" s="10" t="e">
         <f t="shared" ref="AE3:AI8" si="0">P3/D3</f>
-        <v>0</v>
-      </c>
-      <c r="AF3" s="11">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF3" s="11" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG3" s="11" t="e">
         <f t="shared" si="0"/>
@@ -5368,11 +4765,11 @@
       </c>
       <c r="AJ3" s="10">
         <f t="shared" ref="AJ3:AN8" si="1">P3-D3</f>
-        <v>-3.6869999999999998</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="11">
         <f t="shared" si="1"/>
-        <v>-3.6869999999999998</v>
+        <v>0</v>
       </c>
       <c r="AL3" s="11" t="e">
         <f t="shared" si="1"/>
@@ -5408,11 +4805,11 @@
       </c>
       <c r="AT3" s="10">
         <f t="shared" ref="AT3:AX8" si="3">J3 - P3</f>
-        <v>2.6920000000000002</v>
+        <v>0</v>
       </c>
       <c r="AU3" s="11">
         <f t="shared" si="3"/>
-        <v>3.3679999999999999</v>
+        <v>0</v>
       </c>
       <c r="AV3" s="11" t="e">
         <f t="shared" si="3"/>
@@ -5429,30 +4826,30 @@
     </row>
     <row r="4" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C4" s="23" cm="1">
         <f t="array" ref="C4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="21" cm="1">
         <f t="array" ref="D4">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.7130000000000001</v>
+        <v>0</v>
       </c>
       <c r="E4" s="21" cm="1">
         <f t="array" ref="E4">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.7130000000000001</v>
-      </c>
-      <c r="F4" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21" t="e" cm="1">
         <f t="array" ref="F4">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.7130000000000001</v>
-      </c>
-      <c r="G4" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" s="21" t="e" cm="1">
         <f t="array" ref="G4">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.7130000000000001</v>
+        <v>#NUM!</v>
       </c>
       <c r="H4" s="24" t="e" cm="1">
         <f t="array" ref="H4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5460,27 +4857,27 @@
       </c>
       <c r="I4" s="21" cm="1">
         <f t="array" ref="I4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="21" cm="1">
         <f t="array" ref="J4">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="K4" s="21" cm="1">
         <f t="array" ref="K4">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.3719999999999999</v>
-      </c>
-      <c r="L4" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21" t="e" cm="1">
         <f t="array" ref="L4">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.5759999999999996</v>
-      </c>
-      <c r="M4" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="21" t="e" cm="1">
         <f t="array" ref="M4">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.5759999999999996</v>
-      </c>
-      <c r="N4" s="24" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N4" s="24" t="e" cm="1">
         <f t="array" ref="N4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.1257139956489837</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O4" s="21" cm="1">
         <f t="array" ref="O4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5506,21 +4903,21 @@
         <f t="array" ref="T4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U4" s="40">
+      <c r="U4" s="40" t="e">
         <f t="shared" ref="U4:U7" si="4">J4/D4</f>
-        <v>1.0246959085882785</v>
-      </c>
-      <c r="V4" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V4" s="3" t="e">
         <f t="shared" ref="V4:Y7" si="5">K4/E4</f>
-        <v>1.6115001842978252</v>
-      </c>
-      <c r="W4" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W4" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.3180980464430518</v>
-      </c>
-      <c r="X4" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X4" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.3180980464430518</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y4" s="4" t="e">
         <f t="shared" si="5"/>
@@ -5528,31 +4925,31 @@
       </c>
       <c r="Z4" s="34">
         <f t="shared" ref="Z4:Z8" si="6">J4-D4</f>
-        <v>6.6999999999999726E-2</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="32">
         <f t="shared" ref="AA4:AA8" si="7">K4-E4</f>
-        <v>1.6589999999999998</v>
-      </c>
-      <c r="AB4" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="32" t="e">
         <f t="shared" ref="AB4:AB8" si="8">L4-F4</f>
-        <v>0.86299999999999955</v>
-      </c>
-      <c r="AC4" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC4" s="32" t="e">
         <f t="shared" ref="AC4:AC8" si="9">M4-G4</f>
-        <v>0.86299999999999955</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD4" s="35" t="e">
         <f t="shared" ref="AD4:AD8" si="10">N4-H4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE4" s="34">
+      <c r="AE4" s="34" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF4" s="32" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG4" s="32" t="e">
         <f t="shared" si="0"/>
@@ -5568,11 +4965,11 @@
       </c>
       <c r="AJ4" s="34">
         <f t="shared" si="1"/>
-        <v>-2.7130000000000001</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="32">
         <f t="shared" si="1"/>
-        <v>-2.7130000000000001</v>
+        <v>0</v>
       </c>
       <c r="AL4" s="32" t="e">
         <f t="shared" si="1"/>
@@ -5608,11 +5005,11 @@
       </c>
       <c r="AT4" s="34">
         <f t="shared" si="3"/>
-        <v>2.78</v>
+        <v>0</v>
       </c>
       <c r="AU4" s="32">
         <f t="shared" si="3"/>
-        <v>4.3719999999999999</v>
+        <v>0</v>
       </c>
       <c r="AV4" s="32" t="e">
         <f t="shared" si="3"/>
@@ -5629,30 +5026,30 @@
     </row>
     <row r="5" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C5" s="23" cm="1">
         <f t="array" ref="C5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="21" cm="1">
         <f t="array" ref="D5">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.0099999999999998</v>
+        <v>0</v>
       </c>
       <c r="E5" s="21" cm="1">
         <f t="array" ref="E5">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="F5" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="21" t="e" cm="1">
         <f t="array" ref="F5">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="G5" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="21" t="e" cm="1">
         <f t="array" ref="G5">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.0099999999999998</v>
+        <v>#NUM!</v>
       </c>
       <c r="H5" s="24" t="e" cm="1">
         <f t="array" ref="H5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5660,27 +5057,27 @@
       </c>
       <c r="I5" s="21" cm="1">
         <f t="array" ref="I5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" s="21" cm="1">
         <f t="array" ref="J5">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.2370000000000001</v>
+        <v>0</v>
       </c>
       <c r="K5" s="21" cm="1">
         <f t="array" ref="K5">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.52</v>
-      </c>
-      <c r="L5" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21" t="e" cm="1">
         <f t="array" ref="L5">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.8784999999999998</v>
-      </c>
-      <c r="M5" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="21" t="e" cm="1">
         <f t="array" ref="M5">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.8784999999999998</v>
-      </c>
-      <c r="N5" s="24" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N5" s="24" t="e" cm="1">
         <f t="array" ref="N5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>0.90721800026234145</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O5" s="21" cm="1">
         <f t="array" ref="O5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5706,21 +5103,21 @@
         <f t="array" ref="T5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U5" s="40">
+      <c r="U5" s="40" t="e">
         <f t="shared" si="4"/>
-        <v>1.1129353233830848</v>
-      </c>
-      <c r="V5" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V5" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.7512437810945276</v>
-      </c>
-      <c r="W5" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W5" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.432089552238806</v>
-      </c>
-      <c r="X5" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X5" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.432089552238806</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y5" s="4" t="e">
         <f t="shared" si="5"/>
@@ -5728,31 +5125,31 @@
       </c>
       <c r="Z5" s="34">
         <f t="shared" si="6"/>
-        <v>0.22700000000000031</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="32">
         <f t="shared" si="7"/>
-        <v>1.5100000000000002</v>
-      </c>
-      <c r="AB5" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="32" t="e">
         <f t="shared" si="8"/>
-        <v>0.86850000000000005</v>
-      </c>
-      <c r="AC5" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC5" s="32" t="e">
         <f t="shared" si="9"/>
-        <v>0.86850000000000005</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD5" s="35" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE5" s="34">
+      <c r="AE5" s="34" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF5" s="32" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG5" s="32" t="e">
         <f t="shared" si="0"/>
@@ -5768,11 +5165,11 @@
       </c>
       <c r="AJ5" s="34">
         <f t="shared" si="1"/>
-        <v>-2.0099999999999998</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="32">
         <f t="shared" si="1"/>
-        <v>-2.0099999999999998</v>
+        <v>0</v>
       </c>
       <c r="AL5" s="32" t="e">
         <f t="shared" si="1"/>
@@ -5808,11 +5205,11 @@
       </c>
       <c r="AT5" s="34">
         <f t="shared" si="3"/>
-        <v>2.2370000000000001</v>
+        <v>0</v>
       </c>
       <c r="AU5" s="32">
         <f t="shared" si="3"/>
-        <v>3.52</v>
+        <v>0</v>
       </c>
       <c r="AV5" s="32" t="e">
         <f t="shared" si="3"/>
@@ -5829,30 +5226,30 @@
     </row>
     <row r="6" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="23" cm="1">
         <f t="array" ref="C6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="21" cm="1">
         <f t="array" ref="D6">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.8339999999999996</v>
+        <v>0</v>
       </c>
       <c r="E6" s="21" cm="1">
         <f t="array" ref="E6">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.8339999999999996</v>
-      </c>
-      <c r="F6" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21" t="e" cm="1">
         <f t="array" ref="F6">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.8339999999999996</v>
-      </c>
-      <c r="G6" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="21" t="e" cm="1">
         <f t="array" ref="G6">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.8339999999999996</v>
+        <v>#NUM!</v>
       </c>
       <c r="H6" s="24" t="e" cm="1">
         <f t="array" ref="H6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5860,27 +5257,27 @@
       </c>
       <c r="I6" s="21" cm="1">
         <f t="array" ref="I6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="21" cm="1">
         <f t="array" ref="J6">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.0449999999999999</v>
+        <v>0</v>
       </c>
       <c r="K6" s="21" cm="1">
         <f t="array" ref="K6">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>7.29</v>
-      </c>
-      <c r="L6" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21" t="e" cm="1">
         <f t="array" ref="L6">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>5.6675000000000004</v>
-      </c>
-      <c r="M6" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="21" t="e" cm="1">
         <f t="array" ref="M6">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>5.6675000000000004</v>
-      </c>
-      <c r="N6" s="24" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N6" s="24" t="e" cm="1">
         <f t="array" ref="N6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.2945615049503432</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O6" s="21" cm="1">
         <f t="array" ref="O6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -5906,21 +5303,21 @@
         <f t="array" ref="T6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6" s="40">
+      <c r="U6" s="40" t="e">
         <f t="shared" si="4"/>
-        <v>0.83678113363673978</v>
-      </c>
-      <c r="V6" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.5080678527099711</v>
-      </c>
-      <c r="W6" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W6" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.1724244931733556</v>
-      </c>
-      <c r="X6" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X6" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.1724244931733556</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y6" s="4" t="e">
         <f t="shared" si="5"/>
@@ -5928,31 +5325,31 @@
       </c>
       <c r="Z6" s="34">
         <f t="shared" si="6"/>
-        <v>-0.7889999999999997</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="32">
         <f t="shared" si="7"/>
-        <v>2.4560000000000004</v>
-      </c>
-      <c r="AB6" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="32" t="e">
         <f t="shared" si="8"/>
-        <v>0.8335000000000008</v>
-      </c>
-      <c r="AC6" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC6" s="32" t="e">
         <f t="shared" si="9"/>
-        <v>0.8335000000000008</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD6" s="35" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE6" s="34">
+      <c r="AE6" s="34" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF6" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF6" s="32" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG6" s="32" t="e">
         <f t="shared" si="0"/>
@@ -5968,11 +5365,11 @@
       </c>
       <c r="AJ6" s="34">
         <f t="shared" si="1"/>
-        <v>-4.8339999999999996</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="32">
         <f t="shared" si="1"/>
-        <v>-4.8339999999999996</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="32" t="e">
         <f t="shared" si="1"/>
@@ -6008,11 +5405,11 @@
       </c>
       <c r="AT6" s="34">
         <f t="shared" si="3"/>
-        <v>4.0449999999999999</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="32">
         <f t="shared" si="3"/>
-        <v>7.29</v>
+        <v>0</v>
       </c>
       <c r="AV6" s="32" t="e">
         <f t="shared" si="3"/>
@@ -6029,30 +5426,30 @@
     </row>
     <row r="7" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="23" cm="1">
         <f t="array" ref="C7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="21" cm="1">
         <f t="array" ref="D7">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.6639999999999999</v>
+        <v>0</v>
       </c>
       <c r="E7" s="21" cm="1">
         <f t="array" ref="E7">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.6639999999999999</v>
-      </c>
-      <c r="F7" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21" t="e" cm="1">
         <f t="array" ref="F7">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.6639999999999999</v>
-      </c>
-      <c r="G7" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="21" t="e" cm="1">
         <f t="array" ref="G7">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.6639999999999999</v>
+        <v>#NUM!</v>
       </c>
       <c r="H7" s="24" t="e" cm="1">
         <f t="array" ref="H7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -6060,27 +5457,27 @@
       </c>
       <c r="I7" s="21" cm="1">
         <f t="array" ref="I7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="21" cm="1">
         <f t="array" ref="J7">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1.724</v>
+        <v>0</v>
       </c>
       <c r="K7" s="21" cm="1">
         <f t="array" ref="K7">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>3.0129999999999999</v>
-      </c>
-      <c r="L7" s="21" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21" t="e" cm="1">
         <f t="array" ref="L7">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.3685</v>
-      </c>
-      <c r="M7" s="21" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="21" t="e" cm="1">
         <f t="array" ref="M7">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.3685</v>
-      </c>
-      <c r="N7" s="24" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N7" s="24" t="e" cm="1">
         <f t="array" ref="N7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>0.91146064094945889</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O7" s="21" cm="1">
         <f t="array" ref="O7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -6106,21 +5503,21 @@
         <f t="array" ref="T7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U7" s="40">
+      <c r="U7" s="40" t="e">
         <f t="shared" si="4"/>
-        <v>1.0360576923076923</v>
-      </c>
-      <c r="V7" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V7" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.8106971153846154</v>
-      </c>
-      <c r="W7" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W7" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.423377403846154</v>
-      </c>
-      <c r="X7" s="3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X7" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>1.423377403846154</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y7" s="4" t="e">
         <f t="shared" si="5"/>
@@ -6128,31 +5525,31 @@
       </c>
       <c r="Z7" s="34">
         <f t="shared" si="6"/>
-        <v>6.0000000000000053E-2</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="32">
         <f t="shared" si="7"/>
-        <v>1.349</v>
-      </c>
-      <c r="AB7" s="32">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="32" t="e">
         <f t="shared" si="8"/>
-        <v>0.70450000000000013</v>
-      </c>
-      <c r="AC7" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC7" s="32" t="e">
         <f t="shared" si="9"/>
-        <v>0.70450000000000013</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD7" s="35" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE7" s="34">
+      <c r="AE7" s="34" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="32">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF7" s="32" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG7" s="32" t="e">
         <f t="shared" si="0"/>
@@ -6168,11 +5565,11 @@
       </c>
       <c r="AJ7" s="34">
         <f t="shared" si="1"/>
-        <v>-1.6639999999999999</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="32">
         <f t="shared" si="1"/>
-        <v>-1.6639999999999999</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="32" t="e">
         <f t="shared" si="1"/>
@@ -6208,11 +5605,11 @@
       </c>
       <c r="AT7" s="34">
         <f t="shared" si="3"/>
-        <v>1.724</v>
+        <v>0</v>
       </c>
       <c r="AU7" s="32">
         <f t="shared" si="3"/>
-        <v>3.0129999999999999</v>
+        <v>0</v>
       </c>
       <c r="AV7" s="32" t="e">
         <f t="shared" si="3"/>
@@ -6229,30 +5626,30 @@
     </row>
     <row r="8" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C8" s="25" cm="1">
         <f t="array" ref="C8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="26" cm="1">
         <f t="array" ref="D8">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.915</v>
+        <v>0</v>
       </c>
       <c r="E8" s="26" cm="1">
         <f t="array" ref="E8">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.915</v>
-      </c>
-      <c r="F8" s="26" cm="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="26" t="e" cm="1">
         <f t="array" ref="F8">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.915</v>
-      </c>
-      <c r="G8" s="26" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="26" t="e" cm="1">
         <f t="array" ref="G8">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.915</v>
+        <v>#NUM!</v>
       </c>
       <c r="H8" s="27" t="e" cm="1">
         <f t="array" ref="H8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -6260,27 +5657,27 @@
       </c>
       <c r="I8" s="26" cm="1">
         <f t="array" ref="I8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8" s="26" cm="1">
         <f t="array" ref="J8">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>4.74</v>
+        <v>0</v>
       </c>
       <c r="K8" s="26" cm="1">
         <f t="array" ref="K8">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>8.2089999999999996</v>
-      </c>
-      <c r="L8" s="26" cm="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="26" t="e" cm="1">
         <f t="array" ref="L8">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>6.4744999999999999</v>
-      </c>
-      <c r="M8" s="26" cm="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="26" t="e" cm="1">
         <f t="array" ref="M8">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>6.4744999999999999</v>
-      </c>
-      <c r="N8" s="27" cm="1">
+        <v>#NUM!</v>
+      </c>
+      <c r="N8" s="27" t="e" cm="1">
         <f t="array" ref="N8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
-        <v>2.4529534239361337</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O8" s="26" cm="1">
         <f t="array" ref="O8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
@@ -6306,21 +5703,21 @@
         <f t="array" ref="T8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$I$2:$I$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U8" s="41">
+      <c r="U8" s="41" t="e">
         <f t="shared" ref="U8" si="11">J8/D8</f>
-        <v>0.96439471007121058</v>
-      </c>
-      <c r="V8" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V8" s="5" t="e">
         <f t="shared" ref="V8" si="12">K8/E8</f>
-        <v>1.6701932858596134</v>
-      </c>
-      <c r="W8" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W8" s="5" t="e">
         <f t="shared" ref="W8" si="13">L8/F8</f>
-        <v>1.3172939979654119</v>
-      </c>
-      <c r="X8" s="5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X8" s="5" t="e">
         <f t="shared" ref="X8" si="14">M8/G8</f>
-        <v>1.3172939979654119</v>
+        <v>#NUM!</v>
       </c>
       <c r="Y8" s="6" t="e">
         <f t="shared" ref="Y8" si="15">N8/H8</f>
@@ -6328,31 +5725,31 @@
       </c>
       <c r="Z8" s="36">
         <f t="shared" si="6"/>
-        <v>-0.17499999999999982</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="37">
         <f t="shared" si="7"/>
-        <v>3.2939999999999996</v>
-      </c>
-      <c r="AB8" s="37">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="37" t="e">
         <f t="shared" si="8"/>
-        <v>1.5594999999999999</v>
-      </c>
-      <c r="AC8" s="37">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AC8" s="37" t="e">
         <f t="shared" si="9"/>
-        <v>1.5594999999999999</v>
+        <v>#NUM!</v>
       </c>
       <c r="AD8" s="38" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE8" s="36">
+      <c r="AE8" s="36" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AF8" s="37">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AF8" s="37" t="e">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG8" s="37" t="e">
         <f t="shared" si="0"/>
@@ -6368,11 +5765,11 @@
       </c>
       <c r="AJ8" s="36">
         <f t="shared" si="1"/>
-        <v>-4.915</v>
+        <v>0</v>
       </c>
       <c r="AK8" s="37">
         <f t="shared" si="1"/>
-        <v>-4.915</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="37" t="e">
         <f t="shared" si="1"/>
@@ -6408,11 +5805,11 @@
       </c>
       <c r="AT8" s="36">
         <f t="shared" si="3"/>
-        <v>4.74</v>
+        <v>0</v>
       </c>
       <c r="AU8" s="37">
         <f t="shared" si="3"/>
-        <v>8.2089999999999996</v>
+        <v>0</v>
       </c>
       <c r="AV8" s="37" t="e">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Reverted testing configuration for the project_deploy_config.sh script Updated the performance metrics/ibbs-web-app-metrics-combined.xlsx to handle the additional HST date/time column
</commit_message>
<xml_diff>
--- a/performance metrics/ibbs-web-app-metrics-combined.xlsx
+++ b/performance metrics/ibbs-web-app-metrics-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\ibbs-web-app-metrics\performance metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967EE37F-CA3B-4CF9-BB61-DF1D804F0584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7BF83B-4B23-467B-A0B5-7775C42973D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2595" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ibbs-web-app-metrics" sheetId="1" r:id="rId1"/>
@@ -264,13 +264,13 @@
     <t>IBBS_SPEC_DATA_YYYYMMDD.csv</t>
   </si>
   <si>
-    <t>W App Location</t>
-  </si>
-  <si>
     <t>Date/Time (UTC)</t>
   </si>
   <si>
     <t>Date/Time (HST)</t>
+  </si>
+  <si>
+    <t>Web App Location</t>
   </si>
 </sst>
 </file>
@@ -1360,15 +1360,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" style="13" customWidth="1"/>
     <col min="6" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="12"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1379,13 +1380,13 @@
         <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>13</v>
@@ -32035,8 +32036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32277,75 +32278,75 @@
         <v>20</v>
       </c>
       <c r="C3" s="16" cm="1">
-        <f t="array" ref="C3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C3">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D3" s="17" cm="1">
-        <f t="array" ref="D3">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D3">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E3" s="17" cm="1">
-        <f t="array" ref="E3">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E3">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F3" s="17" t="e" cm="1">
-        <f t="array" ref="F3">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F3">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G3" s="17" t="e" cm="1">
-        <f t="array" ref="G3">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G3">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H3" s="18" t="e" cm="1">
-        <f t="array" ref="H3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I3" s="17" cm="1">
-        <f t="array" ref="I3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I3">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J3" s="17" cm="1">
-        <f t="array" ref="J3">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J3">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K3" s="17" cm="1">
-        <f t="array" ref="K3">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K3">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L3" s="17" t="e" cm="1">
-        <f t="array" ref="L3">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L3">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M3" s="17" t="e" cm="1">
-        <f t="array" ref="M3">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M3">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N3" s="18" t="e" cm="1">
-        <f t="array" ref="N3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O3" s="17" cm="1">
-        <f t="array" ref="O3">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O3">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P3" s="17" cm="1">
-        <f t="array" ref="P3">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P3">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q3" s="17" cm="1">
-        <f t="array" ref="Q3">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q3">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R3" s="17" t="e" cm="1">
-        <f t="array" ref="R3">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R3">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S3" s="17" t="e" cm="1">
-        <f t="array" ref="S3">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S3">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T3" s="17" t="e" cm="1">
-        <f t="array" ref="T3">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A3)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U3" s="28" t="e">
@@ -32477,75 +32478,75 @@
         <v>22</v>
       </c>
       <c r="C4" s="21" cm="1">
-        <f t="array" ref="C4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C4">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D4" s="19" cm="1">
-        <f t="array" ref="D4">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D4">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E4" s="19" cm="1">
-        <f t="array" ref="E4">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E4">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F4" s="19" t="e" cm="1">
-        <f t="array" ref="F4">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F4">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G4" s="19" t="e" cm="1">
-        <f t="array" ref="G4">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G4">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H4" s="22" t="e" cm="1">
-        <f t="array" ref="H4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I4" s="19" cm="1">
-        <f t="array" ref="I4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I4">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J4" s="19" cm="1">
-        <f t="array" ref="J4">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J4">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K4" s="19" cm="1">
-        <f t="array" ref="K4">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K4">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L4" s="19" t="e" cm="1">
-        <f t="array" ref="L4">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L4">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M4" s="19" t="e" cm="1">
-        <f t="array" ref="M4">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M4">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N4" s="22" t="e" cm="1">
-        <f t="array" ref="N4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O4" s="19" cm="1">
-        <f t="array" ref="O4">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O4">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P4" s="19" cm="1">
-        <f t="array" ref="P4">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P4">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q4" s="19" cm="1">
-        <f t="array" ref="Q4">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q4">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R4" s="19" t="e" cm="1">
-        <f t="array" ref="R4">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R4">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S4" s="19" t="e" cm="1">
-        <f t="array" ref="S4">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S4">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T4" s="19" t="e" cm="1">
-        <f t="array" ref="T4">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A4)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U4" s="29" t="e">
@@ -32677,75 +32678,75 @@
         <v>23</v>
       </c>
       <c r="C5" s="21" cm="1">
-        <f t="array" ref="C5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C5">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D5" s="19" cm="1">
-        <f t="array" ref="D5">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D5">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E5" s="19" cm="1">
-        <f t="array" ref="E5">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E5">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F5" s="19" t="e" cm="1">
-        <f t="array" ref="F5">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F5">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G5" s="19" t="e" cm="1">
-        <f t="array" ref="G5">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G5">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H5" s="22" t="e" cm="1">
-        <f t="array" ref="H5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I5" s="19" cm="1">
-        <f t="array" ref="I5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I5">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J5" s="19" cm="1">
-        <f t="array" ref="J5">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J5">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K5" s="19" cm="1">
-        <f t="array" ref="K5">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K5">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L5" s="19" t="e" cm="1">
-        <f t="array" ref="L5">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L5">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M5" s="19" t="e" cm="1">
-        <f t="array" ref="M5">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M5">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N5" s="22" t="e" cm="1">
-        <f t="array" ref="N5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O5" s="19" cm="1">
-        <f t="array" ref="O5">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O5">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P5" s="19" cm="1">
-        <f t="array" ref="P5">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P5">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q5" s="19" cm="1">
-        <f t="array" ref="Q5">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q5">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R5" s="19" t="e" cm="1">
-        <f t="array" ref="R5">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R5">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S5" s="19" t="e" cm="1">
-        <f t="array" ref="S5">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S5">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T5" s="19" t="e" cm="1">
-        <f t="array" ref="T5">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A5)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U5" s="29" t="e">
@@ -32877,75 +32878,75 @@
         <v>20</v>
       </c>
       <c r="C6" s="21" cm="1">
-        <f t="array" ref="C6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C6">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D6" s="19" cm="1">
-        <f t="array" ref="D6">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D6">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E6" s="19" cm="1">
-        <f t="array" ref="E6">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E6">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F6" s="19" t="e" cm="1">
-        <f t="array" ref="F6">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F6">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G6" s="19" t="e" cm="1">
-        <f t="array" ref="G6">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G6">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H6" s="22" t="e" cm="1">
-        <f t="array" ref="H6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I6" s="19" cm="1">
-        <f t="array" ref="I6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I6">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J6" s="19" cm="1">
-        <f t="array" ref="J6">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J6">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K6" s="19" cm="1">
-        <f t="array" ref="K6">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K6">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L6" s="19" t="e" cm="1">
-        <f t="array" ref="L6">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L6">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M6" s="19" t="e" cm="1">
-        <f t="array" ref="M6">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M6">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N6" s="22" t="e" cm="1">
-        <f t="array" ref="N6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O6" s="19" cm="1">
-        <f t="array" ref="O6">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O6">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P6" s="19" cm="1">
-        <f t="array" ref="P6">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P6">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q6" s="19" cm="1">
-        <f t="array" ref="Q6">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q6">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R6" s="19" t="e" cm="1">
-        <f t="array" ref="R6">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R6">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S6" s="19" t="e" cm="1">
-        <f t="array" ref="S6">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S6">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T6" s="19" t="e" cm="1">
-        <f t="array" ref="T6">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A6)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U6" s="29" t="e">
@@ -33077,75 +33078,75 @@
         <v>20</v>
       </c>
       <c r="C7" s="21" cm="1">
-        <f t="array" ref="C7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C7">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D7" s="19" cm="1">
-        <f t="array" ref="D7">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D7">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E7" s="19" cm="1">
-        <f t="array" ref="E7">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E7">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F7" s="19" t="e" cm="1">
-        <f t="array" ref="F7">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F7">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G7" s="19" t="e" cm="1">
-        <f t="array" ref="G7">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G7">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H7" s="22" t="e" cm="1">
-        <f t="array" ref="H7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I7" s="19" cm="1">
-        <f t="array" ref="I7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I7">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J7" s="19" cm="1">
-        <f t="array" ref="J7">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J7">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K7" s="19" cm="1">
-        <f t="array" ref="K7">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K7">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L7" s="19" t="e" cm="1">
-        <f t="array" ref="L7">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L7">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M7" s="19" t="e" cm="1">
-        <f t="array" ref="M7">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M7">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N7" s="22" t="e" cm="1">
-        <f t="array" ref="N7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O7" s="19" cm="1">
-        <f t="array" ref="O7">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O7">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P7" s="19" cm="1">
-        <f t="array" ref="P7">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P7">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q7" s="19" cm="1">
-        <f t="array" ref="Q7">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q7">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R7" s="19" t="e" cm="1">
-        <f t="array" ref="R7">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R7">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="19" t="e" cm="1">
-        <f t="array" ref="S7">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S7">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T7" s="19" t="e" cm="1">
-        <f t="array" ref="T7">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A7)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U7" s="29" t="e">
@@ -33277,75 +33278,75 @@
         <v>26</v>
       </c>
       <c r="C8" s="21" cm="1">
-        <f t="array" ref="C8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C8">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D8" s="19" cm="1">
-        <f t="array" ref="D8">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D8">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E8" s="19" cm="1">
-        <f t="array" ref="E8">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E8">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F8" s="19" t="e" cm="1">
-        <f t="array" ref="F8">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F8">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G8" s="19" t="e" cm="1">
-        <f t="array" ref="G8">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G8">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H8" s="22" t="e" cm="1">
-        <f t="array" ref="H8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I8" s="19" cm="1">
-        <f t="array" ref="I8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I8">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J8" s="19" cm="1">
-        <f t="array" ref="J8">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J8">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K8" s="19" cm="1">
-        <f t="array" ref="K8">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K8">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L8" s="19" t="e" cm="1">
-        <f t="array" ref="L8">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L8">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M8" s="19" t="e" cm="1">
-        <f t="array" ref="M8">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M8">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N8" s="22" t="e" cm="1">
-        <f t="array" ref="N8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O8" s="19" cm="1">
-        <f t="array" ref="O8">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O8">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P8" s="19" cm="1">
-        <f t="array" ref="P8">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P8">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q8" s="19" cm="1">
-        <f t="array" ref="Q8">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q8">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R8" s="19" t="e" cm="1">
-        <f t="array" ref="R8">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R8">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S8" s="19" t="e" cm="1">
-        <f t="array" ref="S8">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S8">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T8" s="19" t="e" cm="1">
-        <f t="array" ref="T8">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A8)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U8" s="29" t="e">
@@ -33477,75 +33478,75 @@
         <v>26</v>
       </c>
       <c r="C9" s="21" cm="1">
-        <f t="array" ref="C9">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C9">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D9" s="19" cm="1">
-        <f t="array" ref="D9">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D9">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E9" s="19" cm="1">
-        <f t="array" ref="E9">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E9">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F9" s="19" t="e" cm="1">
-        <f t="array" ref="F9">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F9">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G9" s="19" t="e" cm="1">
-        <f t="array" ref="G9">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G9">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H9" s="22" t="e" cm="1">
-        <f t="array" ref="H9">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I9" s="19" cm="1">
-        <f t="array" ref="I9">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I9">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J9" s="19" cm="1">
-        <f t="array" ref="J9">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J9">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K9" s="19" cm="1">
-        <f t="array" ref="K9">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K9">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L9" s="19" t="e" cm="1">
-        <f t="array" ref="L9">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L9">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M9" s="19" t="e" cm="1">
-        <f t="array" ref="M9">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M9">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N9" s="22" t="e" cm="1">
-        <f t="array" ref="N9">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O9" s="19" cm="1">
-        <f t="array" ref="O9">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O9">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P9" s="19" cm="1">
-        <f t="array" ref="P9">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P9">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q9" s="19" cm="1">
-        <f t="array" ref="Q9">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q9">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R9" s="19" t="e" cm="1">
-        <f t="array" ref="R9">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R9">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S9" s="19" t="e" cm="1">
-        <f t="array" ref="S9">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S9">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T9" s="22" t="e" cm="1">
-        <f t="array" ref="T9">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A9)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U9" s="3" t="e">
@@ -33677,75 +33678,75 @@
         <v>31</v>
       </c>
       <c r="C10" s="21" cm="1">
-        <f t="array" ref="C10">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C10">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D10" s="19" cm="1">
-        <f t="array" ref="D10">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D10">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E10" s="19" cm="1">
-        <f t="array" ref="E10">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E10">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F10" s="19" t="e" cm="1">
-        <f t="array" ref="F10">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F10">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G10" s="19" t="e" cm="1">
-        <f t="array" ref="G10">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G10">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H10" s="22" t="e" cm="1">
-        <f t="array" ref="H10">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I10" s="19" cm="1">
-        <f t="array" ref="I10">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I10">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J10" s="19" cm="1">
-        <f t="array" ref="J10">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J10">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K10" s="19" cm="1">
-        <f t="array" ref="K10">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K10">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L10" s="19" t="e" cm="1">
-        <f t="array" ref="L10">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L10">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="19" t="e" cm="1">
-        <f t="array" ref="M10">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M10">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N10" s="22" t="e" cm="1">
-        <f t="array" ref="N10">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O10" s="19" cm="1">
-        <f t="array" ref="O10">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O10">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P10" s="19" cm="1">
-        <f t="array" ref="P10">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P10">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q10" s="19" cm="1">
-        <f t="array" ref="Q10">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q10">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R10" s="19" t="e" cm="1">
-        <f t="array" ref="R10">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R10">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S10" s="19" t="e" cm="1">
-        <f t="array" ref="S10">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S10">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T10" s="22" t="e" cm="1">
-        <f t="array" ref="T10">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A10)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U10" s="3" t="e">
@@ -33877,75 +33878,75 @@
         <v>20</v>
       </c>
       <c r="C11" s="21" cm="1">
-        <f t="array" ref="C11">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C11">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D11" s="19" cm="1">
-        <f t="array" ref="D11">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D11">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E11" s="19" cm="1">
-        <f t="array" ref="E11">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E11">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F11" s="19" t="e" cm="1">
-        <f t="array" ref="F11">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F11">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G11" s="19" t="e" cm="1">
-        <f t="array" ref="G11">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G11">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H11" s="22" t="e" cm="1">
-        <f t="array" ref="H11">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I11" s="19" cm="1">
-        <f t="array" ref="I11">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I11">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J11" s="19" cm="1">
-        <f t="array" ref="J11">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J11">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K11" s="19" cm="1">
-        <f t="array" ref="K11">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K11">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L11" s="19" t="e" cm="1">
-        <f t="array" ref="L11">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L11">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="19" t="e" cm="1">
-        <f t="array" ref="M11">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M11">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N11" s="22" t="e" cm="1">
-        <f t="array" ref="N11">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O11" s="19" cm="1">
-        <f t="array" ref="O11">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O11">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P11" s="19" cm="1">
-        <f t="array" ref="P11">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P11">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q11" s="19" cm="1">
-        <f t="array" ref="Q11">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q11">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R11" s="19" t="e" cm="1">
-        <f t="array" ref="R11">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R11">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="19" t="e" cm="1">
-        <f t="array" ref="S11">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S11">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T11" s="22" t="e" cm="1">
-        <f t="array" ref="T11">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A11)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U11" s="3" t="e">
@@ -34077,75 +34078,75 @@
         <v>23</v>
       </c>
       <c r="C12" s="21" cm="1">
-        <f t="array" ref="C12">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="C12">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="D12" s="19" cm="1">
-        <f t="array" ref="D12">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="D12">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="E12" s="19" cm="1">
-        <f t="array" ref="E12">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="E12">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="F12" s="19" t="e" cm="1">
-        <f t="array" ref="F12">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="F12">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G12" s="19" t="e" cm="1">
-        <f t="array" ref="G12">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="G12">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="H12" s="22" t="e" cm="1">
-        <f t="array" ref="H12">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="H12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="I12" s="19" cm="1">
-        <f t="array" ref="I12">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="I12">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="J12" s="19" cm="1">
-        <f t="array" ref="J12">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="J12">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="K12" s="19" cm="1">
-        <f t="array" ref="K12">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="K12">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="L12" s="19" t="e" cm="1">
-        <f t="array" ref="L12">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="L12">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="19" t="e" cm="1">
-        <f t="array" ref="M12">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="M12">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="N12" s="22" t="e" cm="1">
-        <f t="array" ref="N12">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="N12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O12" s="19" cm="1">
-        <f t="array" ref="O12">COUNT(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="O12">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="P12" s="19" cm="1">
-        <f t="array" ref="P12">MIN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="P12">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="Q12" s="19" cm="1">
-        <f t="array" ref="Q12">MAX(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="Q12">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>0</v>
       </c>
       <c r="R12" s="19" t="e" cm="1">
-        <f t="array" ref="R12">AVERAGE(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="R12">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="19" t="e" cm="1">
-        <f t="array" ref="S12">MEDIAN(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="S12">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#NUM!</v>
       </c>
       <c r="T12" s="22" t="e" cm="1">
-        <f t="array" ref="T12">STDEV(IF(('ibbs-web-app-metrics'!$E$2:$E$9999=$A12)*('ibbs-web-app-metrics'!$F$2:$F$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
+        <f t="array" ref="T12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="U12" s="3" t="e">

</xml_diff>

<commit_message>
Updated the project to add more scenarios
</commit_message>
<xml_diff>
--- a/performance metrics/ibbs-web-app-metrics-combined.xlsx
+++ b/performance metrics/ibbs-web-app-metrics-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\ibbs-web-app-metrics\performance metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE7BF83B-4B23-467B-A0B5-7775C42973D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0D49EE-D7F1-455D-9B2D-6CEE72E63889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ibbs-web-app-metrics" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="48">
   <si>
     <t>Local</t>
   </si>
@@ -271,6 +271,39 @@
   </si>
   <si>
     <t>Web App Location</t>
+  </si>
+  <si>
+    <t>IBBS APEX app</t>
+  </si>
+  <si>
+    <t>Login.png</t>
+  </si>
+  <si>
+    <t>Full Sampling Plan Report.png</t>
+  </si>
+  <si>
+    <t>Full Sampling Plan Report filter.png</t>
+  </si>
+  <si>
+    <t>View Specimens.png</t>
+  </si>
+  <si>
+    <t>View Edit Specimen.png</t>
+  </si>
+  <si>
+    <t>View Edit Specimen post specimen record insert.png</t>
+  </si>
+  <si>
+    <t>View Specimens post specimen record update.png</t>
+  </si>
+  <si>
+    <t>View Specimens specimen download complete.png</t>
+  </si>
+  <si>
+    <t>Sampling Plan Summary Region Report.png</t>
+  </si>
+  <si>
+    <t>Sampling Plan Summary Region Report filter.png</t>
   </si>
 </sst>
 </file>
@@ -1353,9 +1386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" sqref="A1:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,111 +1441,746 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E2" s="15"/>
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15">
+        <v>45560.930810185186</v>
+      </c>
+      <c r="E2" s="15">
+        <v>45560.514143518521</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="12">
+        <v>25</v>
+      </c>
+      <c r="I2">
+        <v>1682.94</v>
+      </c>
+      <c r="J2">
+        <v>5.7720000000000002</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E3" s="15"/>
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="15">
+        <v>45560.930891203701</v>
+      </c>
+      <c r="E3" s="15">
+        <v>45560.514224537037</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12">
+        <v>41</v>
+      </c>
+      <c r="I3">
+        <v>3799.84</v>
+      </c>
+      <c r="J3">
+        <v>3.3759999999999999</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E4" s="15"/>
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15">
+        <v>45560.930937500001</v>
+      </c>
+      <c r="E4" s="15">
+        <v>45560.514270833337</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="12">
+        <v>41</v>
+      </c>
+      <c r="I4">
+        <v>3800.15</v>
+      </c>
+      <c r="J4">
+        <v>2.2410000000000001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E5" s="15"/>
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="15">
+        <v>45560.930960648147</v>
+      </c>
+      <c r="E5" s="15">
+        <v>45560.514293981483</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>34</v>
+      </c>
+      <c r="I5">
+        <v>4538.41</v>
+      </c>
+      <c r="J5">
+        <v>5.8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E6" s="15"/>
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15">
+        <v>45560.931041666663</v>
+      </c>
+      <c r="E6" s="15">
+        <v>45560.514374999999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="12">
+        <v>35</v>
+      </c>
+      <c r="I6">
+        <v>3131.02</v>
+      </c>
+      <c r="J6">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E7" s="15"/>
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="15">
+        <v>45560.931180555555</v>
+      </c>
+      <c r="E7" s="15">
+        <v>45560.514513888891</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="12">
+        <v>54</v>
+      </c>
+      <c r="I7">
+        <v>3827.29</v>
+      </c>
+      <c r="J7">
+        <v>2.4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E8" s="15"/>
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15">
+        <v>45560.931261574071</v>
+      </c>
+      <c r="E8" s="15">
+        <v>45560.514594907407</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="12">
+        <v>40</v>
+      </c>
+      <c r="I8">
+        <v>4546.8599999999997</v>
+      </c>
+      <c r="J8">
+        <v>5.6360000000000001</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E9" s="15"/>
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <v>45560.931331018517</v>
+      </c>
+      <c r="E9" s="15">
+        <v>45560.514664351853</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="12">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1811934</v>
+      </c>
+      <c r="J9">
+        <v>2.532</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E10" s="15"/>
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="15">
+        <v>45560.93136574074</v>
+      </c>
+      <c r="E10" s="15">
+        <v>45560.514699074076</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="12">
+        <v>47</v>
+      </c>
+      <c r="I10">
+        <v>5405.12</v>
+      </c>
+      <c r="J10">
+        <v>5.4189999999999996</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="H11"/>
-      <c r="I11" s="12"/>
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="15">
+        <v>45560.931435185186</v>
+      </c>
+      <c r="E11" s="15">
+        <v>45560.514768518522</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>46</v>
+      </c>
+      <c r="I11" s="12">
+        <v>5168.3500000000004</v>
+      </c>
+      <c r="J11">
+        <v>4.5259999999999998</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="15"/>
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
+        <v>45560.934305555558</v>
+      </c>
+      <c r="E12" s="15">
+        <v>45560.517638888887</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="12">
+        <v>26</v>
+      </c>
+      <c r="I12">
+        <v>745.47</v>
+      </c>
+      <c r="J12">
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E13" s="15"/>
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
+        <v>45560.934351851851</v>
+      </c>
+      <c r="E13" s="15">
+        <v>45560.517685185187</v>
+      </c>
+      <c r="F13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="12">
+        <v>40</v>
+      </c>
+      <c r="I13">
+        <v>1158.8399999999999</v>
+      </c>
+      <c r="J13">
+        <v>3.6749999999999998</v>
+      </c>
+      <c r="K13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E14" s="15"/>
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15">
+        <v>45560.934398148151</v>
+      </c>
+      <c r="E14" s="15">
+        <v>45560.517731481479</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="12">
+        <v>40</v>
+      </c>
+      <c r="I14">
+        <v>1158.8599999999999</v>
+      </c>
+      <c r="J14">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="K14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="15"/>
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
+        <v>45560.934432870374</v>
+      </c>
+      <c r="E15" s="15">
+        <v>45560.517766203702</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="12">
+        <v>35</v>
+      </c>
+      <c r="I15">
+        <v>1391.29</v>
+      </c>
+      <c r="J15">
+        <v>7.1150000000000002</v>
+      </c>
+      <c r="K15" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="15"/>
-      <c r="H20"/>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="15"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
+        <v>45560.934525462966</v>
+      </c>
+      <c r="E16" s="15">
+        <v>45560.517858796295</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="12">
+        <v>33</v>
+      </c>
+      <c r="I16">
+        <v>911.34</v>
+      </c>
+      <c r="J16">
+        <v>3.7989999999999999</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15">
+        <v>45560.934699074074</v>
+      </c>
+      <c r="E17" s="15">
+        <v>45560.51803240741</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="12">
+        <v>53</v>
+      </c>
+      <c r="I17">
+        <v>1174.57</v>
+      </c>
+      <c r="J17">
+        <v>4.8840000000000003</v>
+      </c>
+      <c r="K17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="15">
+        <v>45560.934907407405</v>
+      </c>
+      <c r="E18" s="15">
+        <v>45560.518240740741</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="12">
+        <v>41</v>
+      </c>
+      <c r="I18">
+        <v>1392.18</v>
+      </c>
+      <c r="J18">
+        <v>6.8319999999999999</v>
+      </c>
+      <c r="K18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="15">
+        <v>45560.934999999998</v>
+      </c>
+      <c r="E19" s="15">
+        <v>45560.518333333333</v>
+      </c>
+      <c r="F19" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1804315</v>
+      </c>
+      <c r="J19">
+        <v>3.1619999999999999</v>
+      </c>
+      <c r="K19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="15">
+        <v>45560.935046296298</v>
+      </c>
+      <c r="E20" s="15">
+        <v>45560.518379629626</v>
+      </c>
+      <c r="F20" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20">
+        <v>44</v>
+      </c>
+      <c r="I20">
+        <v>1512.01</v>
+      </c>
+      <c r="J20">
+        <v>5.2069999999999999</v>
+      </c>
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="15">
+        <v>45560.93513888889</v>
+      </c>
+      <c r="E21" s="15">
+        <v>45560.518472222226</v>
+      </c>
+      <c r="F21" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>48</v>
+      </c>
+      <c r="I21">
+        <v>1516.82</v>
+      </c>
+      <c r="J21">
+        <v>5.5060000000000002</v>
+      </c>
+      <c r="K21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E22" s="15"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E23" s="15"/>
       <c r="H23"/>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E24" s="15"/>
       <c r="H24"/>
     </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E25" s="15"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E26" s="15"/>
       <c r="H26"/>
     </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E27" s="15"/>
       <c r="H27"/>
     </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E28" s="15"/>
       <c r="H28"/>
     </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E29" s="15"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E30" s="15"/>
       <c r="H30"/>
     </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E31" s="15"/>
       <c r="H31"/>
     </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E32" s="15"/>
       <c r="H32"/>
     </row>
@@ -32036,8 +32704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32279,23 +32947,23 @@
       </c>
       <c r="C3" s="16" cm="1">
         <f t="array" ref="C3">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="17" cm="1">
         <f t="array" ref="D3">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.7720000000000002</v>
       </c>
       <c r="E3" s="17" cm="1">
         <f t="array" ref="E3">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="17" t="e" cm="1">
+        <v>5.7720000000000002</v>
+      </c>
+      <c r="F3" s="17" cm="1">
         <f t="array" ref="F3">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G3" s="17" t="e" cm="1">
+        <v>5.7720000000000002</v>
+      </c>
+      <c r="G3" s="17" cm="1">
         <f t="array" ref="G3">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.7720000000000002</v>
       </c>
       <c r="H3" s="18" t="e" cm="1">
         <f t="array" ref="H3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32303,23 +32971,23 @@
       </c>
       <c r="I3" s="17" cm="1">
         <f t="array" ref="I3">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="17" cm="1">
         <f t="array" ref="J3">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>2.7370000000000001</v>
       </c>
       <c r="K3" s="17" cm="1">
         <f t="array" ref="K3">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L3" s="17" t="e" cm="1">
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="L3" s="17" cm="1">
         <f t="array" ref="L3">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" s="17" t="e" cm="1">
+        <v>2.7370000000000001</v>
+      </c>
+      <c r="M3" s="17" cm="1">
         <f t="array" ref="M3">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>2.7370000000000001</v>
       </c>
       <c r="N3" s="18" t="e" cm="1">
         <f t="array" ref="N3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32349,21 +33017,21 @@
         <f t="array" ref="T3">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A3)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B3)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U3" s="28" t="e">
+      <c r="U3" s="28">
         <f>J3/D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V3" s="6" t="e">
+        <v>0.47418572418572419</v>
+      </c>
+      <c r="V3" s="6">
         <f>K3/E3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W3" s="6" t="e">
+        <v>0.47418572418572419</v>
+      </c>
+      <c r="W3" s="6">
         <f>L3/F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X3" s="6" t="e">
+        <v>0.47418572418572419</v>
+      </c>
+      <c r="X3" s="6">
         <f>M3/G3</f>
-        <v>#NUM!</v>
+        <v>0.47418572418572419</v>
       </c>
       <c r="Y3" s="7" t="e">
         <f>N3/H3</f>
@@ -32371,31 +33039,31 @@
       </c>
       <c r="Z3" s="8">
         <f>J3-D3</f>
-        <v>0</v>
+        <v>-3.0350000000000001</v>
       </c>
       <c r="AA3" s="9">
         <f>K3-E3</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="9" t="e">
+        <v>-3.0350000000000001</v>
+      </c>
+      <c r="AB3" s="9">
         <f>L3-F3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC3" s="9" t="e">
+        <v>-3.0350000000000001</v>
+      </c>
+      <c r="AC3" s="9">
         <f>M3-G3</f>
-        <v>#NUM!</v>
+        <v>-3.0350000000000001</v>
       </c>
       <c r="AD3" s="10" t="e">
         <f>N3-H3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE3" s="8" t="e">
+      <c r="AE3" s="8">
         <f t="shared" ref="AE3:AI8" si="0">P3/D3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF3" s="9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG3" s="9" t="e">
         <f t="shared" si="0"/>
@@ -32411,11 +33079,11 @@
       </c>
       <c r="AJ3" s="8">
         <f t="shared" ref="AJ3:AN8" si="1">P3-D3</f>
-        <v>0</v>
+        <v>-5.7720000000000002</v>
       </c>
       <c r="AK3" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5.7720000000000002</v>
       </c>
       <c r="AL3" s="9" t="e">
         <f t="shared" si="1"/>
@@ -32451,11 +33119,11 @@
       </c>
       <c r="AT3" s="8">
         <f t="shared" ref="AT3:AX8" si="3">J3 - P3</f>
-        <v>0</v>
+        <v>2.7370000000000001</v>
       </c>
       <c r="AU3" s="9">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.7370000000000001</v>
       </c>
       <c r="AV3" s="9" t="e">
         <f t="shared" si="3"/>
@@ -32479,23 +33147,23 @@
       </c>
       <c r="C4" s="21" cm="1">
         <f t="array" ref="C4">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="19" cm="1">
         <f t="array" ref="D4">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>3.3759999999999999</v>
       </c>
       <c r="E4" s="19" cm="1">
         <f t="array" ref="E4">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="19" t="e" cm="1">
+        <v>3.3759999999999999</v>
+      </c>
+      <c r="F4" s="19" cm="1">
         <f t="array" ref="F4">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G4" s="19" t="e" cm="1">
+        <v>3.3759999999999999</v>
+      </c>
+      <c r="G4" s="19" cm="1">
         <f t="array" ref="G4">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>3.3759999999999999</v>
       </c>
       <c r="H4" s="22" t="e" cm="1">
         <f t="array" ref="H4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32503,23 +33171,23 @@
       </c>
       <c r="I4" s="19" cm="1">
         <f t="array" ref="I4">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="19" cm="1">
         <f t="array" ref="J4">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="K4" s="19" cm="1">
         <f t="array" ref="K4">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="19" t="e" cm="1">
+        <v>3.6749999999999998</v>
+      </c>
+      <c r="L4" s="19" cm="1">
         <f t="array" ref="L4">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" s="19" t="e" cm="1">
+        <v>3.6749999999999998</v>
+      </c>
+      <c r="M4" s="19" cm="1">
         <f t="array" ref="M4">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="N4" s="22" t="e" cm="1">
         <f t="array" ref="N4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32549,21 +33217,21 @@
         <f t="array" ref="T4">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A4)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B4)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U4" s="29" t="e">
+      <c r="U4" s="29">
         <f t="shared" ref="U4:U7" si="4">J4/D4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V4" s="3" t="e">
+        <v>1.0885663507109005</v>
+      </c>
+      <c r="V4" s="3">
         <f t="shared" ref="V4:Y7" si="5">K4/E4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W4" s="3" t="e">
+        <v>1.0885663507109005</v>
+      </c>
+      <c r="W4" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X4" s="3" t="e">
+        <v>1.0885663507109005</v>
+      </c>
+      <c r="X4" s="3">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
+        <v>1.0885663507109005</v>
       </c>
       <c r="Y4" s="4" t="e">
         <f t="shared" si="5"/>
@@ -32571,31 +33239,31 @@
       </c>
       <c r="Z4" s="26">
         <f t="shared" ref="Z4:Z8" si="6">J4-D4</f>
-        <v>0</v>
+        <v>0.29899999999999993</v>
       </c>
       <c r="AA4" s="24">
         <f t="shared" ref="AA4:AA8" si="7">K4-E4</f>
-        <v>0</v>
-      </c>
-      <c r="AB4" s="24" t="e">
+        <v>0.29899999999999993</v>
+      </c>
+      <c r="AB4" s="24">
         <f t="shared" ref="AB4:AB8" si="8">L4-F4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC4" s="24" t="e">
+        <v>0.29899999999999993</v>
+      </c>
+      <c r="AC4" s="24">
         <f t="shared" ref="AC4:AC8" si="9">M4-G4</f>
-        <v>#NUM!</v>
+        <v>0.29899999999999993</v>
       </c>
       <c r="AD4" s="27" t="e">
         <f t="shared" ref="AD4:AD8" si="10">N4-H4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE4" s="26" t="e">
+      <c r="AE4" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF4" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="24" t="e">
         <f t="shared" si="0"/>
@@ -32611,11 +33279,11 @@
       </c>
       <c r="AJ4" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3.3759999999999999</v>
       </c>
       <c r="AK4" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3.3759999999999999</v>
       </c>
       <c r="AL4" s="24" t="e">
         <f t="shared" si="1"/>
@@ -32651,11 +33319,11 @@
       </c>
       <c r="AT4" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="AU4" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.6749999999999998</v>
       </c>
       <c r="AV4" s="24" t="e">
         <f t="shared" si="3"/>
@@ -32679,23 +33347,23 @@
       </c>
       <c r="C5" s="21" cm="1">
         <f t="array" ref="C5">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="19" cm="1">
         <f t="array" ref="D5">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>2.2410000000000001</v>
       </c>
       <c r="E5" s="19" cm="1">
         <f t="array" ref="E5">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="19" t="e" cm="1">
+        <v>2.2410000000000001</v>
+      </c>
+      <c r="F5" s="19" cm="1">
         <f t="array" ref="F5">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G5" s="19" t="e" cm="1">
+        <v>2.2410000000000001</v>
+      </c>
+      <c r="G5" s="19" cm="1">
         <f t="array" ref="G5">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>2.2410000000000001</v>
       </c>
       <c r="H5" s="22" t="e" cm="1">
         <f t="array" ref="H5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32703,23 +33371,23 @@
       </c>
       <c r="I5" s="19" cm="1">
         <f t="array" ref="I5">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="19" cm="1">
         <f t="array" ref="J5">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="K5" s="19" cm="1">
         <f t="array" ref="K5">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="19" t="e" cm="1">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="L5" s="19" cm="1">
         <f t="array" ref="L5">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="19" t="e" cm="1">
+        <v>2.2250000000000001</v>
+      </c>
+      <c r="M5" s="19" cm="1">
         <f t="array" ref="M5">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="N5" s="22" t="e" cm="1">
         <f t="array" ref="N5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32749,21 +33417,21 @@
         <f t="array" ref="T5">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A5)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B5)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U5" s="29" t="e">
+      <c r="U5" s="29">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V5" s="3" t="e">
+        <v>0.99286033020972775</v>
+      </c>
+      <c r="V5" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W5" s="3" t="e">
+        <v>0.99286033020972775</v>
+      </c>
+      <c r="W5" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X5" s="3" t="e">
+        <v>0.99286033020972775</v>
+      </c>
+      <c r="X5" s="3">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
+        <v>0.99286033020972775</v>
       </c>
       <c r="Y5" s="4" t="e">
         <f t="shared" si="5"/>
@@ -32771,31 +33439,31 @@
       </c>
       <c r="Z5" s="26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1.6000000000000014E-2</v>
       </c>
       <c r="AA5" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="24" t="e">
+        <v>-1.6000000000000014E-2</v>
+      </c>
+      <c r="AB5" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC5" s="24" t="e">
+        <v>-1.6000000000000014E-2</v>
+      </c>
+      <c r="AC5" s="24">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>-1.6000000000000014E-2</v>
       </c>
       <c r="AD5" s="27" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE5" s="26" t="e">
+      <c r="AE5" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF5" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG5" s="24" t="e">
         <f t="shared" si="0"/>
@@ -32811,11 +33479,11 @@
       </c>
       <c r="AJ5" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.2410000000000001</v>
       </c>
       <c r="AK5" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.2410000000000001</v>
       </c>
       <c r="AL5" s="24" t="e">
         <f t="shared" si="1"/>
@@ -32851,11 +33519,11 @@
       </c>
       <c r="AT5" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="AU5" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.2250000000000001</v>
       </c>
       <c r="AV5" s="24" t="e">
         <f t="shared" si="3"/>
@@ -32879,23 +33547,23 @@
       </c>
       <c r="C6" s="21" cm="1">
         <f t="array" ref="C6">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="19" cm="1">
         <f t="array" ref="D6">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.8</v>
       </c>
       <c r="E6" s="19" cm="1">
         <f t="array" ref="E6">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="19" t="e" cm="1">
+        <v>5.8</v>
+      </c>
+      <c r="F6" s="19" cm="1">
         <f t="array" ref="F6">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G6" s="19" t="e" cm="1">
+        <v>5.8</v>
+      </c>
+      <c r="G6" s="19" cm="1">
         <f t="array" ref="G6">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.8</v>
       </c>
       <c r="H6" s="22" t="e" cm="1">
         <f t="array" ref="H6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32903,23 +33571,23 @@
       </c>
       <c r="I6" s="19" cm="1">
         <f t="array" ref="I6">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="19" cm="1">
         <f t="array" ref="J6">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="K6" s="19" cm="1">
         <f t="array" ref="K6">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="19" t="e" cm="1">
+        <v>7.1150000000000002</v>
+      </c>
+      <c r="L6" s="19" cm="1">
         <f t="array" ref="L6">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M6" s="19" t="e" cm="1">
+        <v>7.1150000000000002</v>
+      </c>
+      <c r="M6" s="19" cm="1">
         <f t="array" ref="M6">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="N6" s="22" t="e" cm="1">
         <f t="array" ref="N6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -32949,21 +33617,21 @@
         <f t="array" ref="T6">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A6)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B6)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6" s="29" t="e">
+      <c r="U6" s="29">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V6" s="3" t="e">
+        <v>1.2267241379310345</v>
+      </c>
+      <c r="V6" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W6" s="3" t="e">
+        <v>1.2267241379310345</v>
+      </c>
+      <c r="W6" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X6" s="3" t="e">
+        <v>1.2267241379310345</v>
+      </c>
+      <c r="X6" s="3">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
+        <v>1.2267241379310345</v>
       </c>
       <c r="Y6" s="4" t="e">
         <f t="shared" si="5"/>
@@ -32971,31 +33639,31 @@
       </c>
       <c r="Z6" s="26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1.3150000000000004</v>
       </c>
       <c r="AA6" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB6" s="24" t="e">
+        <v>1.3150000000000004</v>
+      </c>
+      <c r="AB6" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC6" s="24" t="e">
+        <v>1.3150000000000004</v>
+      </c>
+      <c r="AC6" s="24">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>1.3150000000000004</v>
       </c>
       <c r="AD6" s="27" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE6" s="26" t="e">
+      <c r="AE6" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF6" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="24" t="e">
         <f t="shared" si="0"/>
@@ -33011,11 +33679,11 @@
       </c>
       <c r="AJ6" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5.8</v>
       </c>
       <c r="AK6" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-5.8</v>
       </c>
       <c r="AL6" s="24" t="e">
         <f t="shared" si="1"/>
@@ -33051,11 +33719,11 @@
       </c>
       <c r="AT6" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="AU6" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.1150000000000002</v>
       </c>
       <c r="AV6" s="24" t="e">
         <f t="shared" si="3"/>
@@ -33079,23 +33747,23 @@
       </c>
       <c r="C7" s="21" cm="1">
         <f t="array" ref="C7">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="19" cm="1">
         <f t="array" ref="D7">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1.7869999999999999</v>
       </c>
       <c r="E7" s="19" cm="1">
         <f t="array" ref="E7">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="19" t="e" cm="1">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="F7" s="19" cm="1">
         <f t="array" ref="F7">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G7" s="19" t="e" cm="1">
+        <v>1.7869999999999999</v>
+      </c>
+      <c r="G7" s="19" cm="1">
         <f t="array" ref="G7">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>1.7869999999999999</v>
       </c>
       <c r="H7" s="22" t="e" cm="1">
         <f t="array" ref="H7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33103,23 +33771,23 @@
       </c>
       <c r="I7" s="19" cm="1">
         <f t="array" ref="I7">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7" s="19" cm="1">
         <f t="array" ref="J7">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>3.7989999999999999</v>
       </c>
       <c r="K7" s="19" cm="1">
         <f t="array" ref="K7">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="19" t="e" cm="1">
+        <v>3.7989999999999999</v>
+      </c>
+      <c r="L7" s="19" cm="1">
         <f t="array" ref="L7">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="19" t="e" cm="1">
+        <v>3.7989999999999999</v>
+      </c>
+      <c r="M7" s="19" cm="1">
         <f t="array" ref="M7">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>3.7989999999999999</v>
       </c>
       <c r="N7" s="22" t="e" cm="1">
         <f t="array" ref="N7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33149,21 +33817,21 @@
         <f t="array" ref="T7">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A7)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B7)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U7" s="29" t="e">
+      <c r="U7" s="29">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V7" s="3" t="e">
+        <v>2.1259093452714048</v>
+      </c>
+      <c r="V7" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W7" s="3" t="e">
+        <v>2.1259093452714048</v>
+      </c>
+      <c r="W7" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X7" s="3" t="e">
+        <v>2.1259093452714048</v>
+      </c>
+      <c r="X7" s="3">
         <f t="shared" si="5"/>
-        <v>#NUM!</v>
+        <v>2.1259093452714048</v>
       </c>
       <c r="Y7" s="4" t="e">
         <f t="shared" si="5"/>
@@ -33171,31 +33839,31 @@
       </c>
       <c r="Z7" s="26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.012</v>
       </c>
       <c r="AA7" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="24" t="e">
+        <v>2.012</v>
+      </c>
+      <c r="AB7" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC7" s="24" t="e">
+        <v>2.012</v>
+      </c>
+      <c r="AC7" s="24">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>2.012</v>
       </c>
       <c r="AD7" s="27" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE7" s="26" t="e">
+      <c r="AE7" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF7" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG7" s="24" t="e">
         <f t="shared" si="0"/>
@@ -33211,11 +33879,11 @@
       </c>
       <c r="AJ7" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.7869999999999999</v>
       </c>
       <c r="AK7" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.7869999999999999</v>
       </c>
       <c r="AL7" s="24" t="e">
         <f t="shared" si="1"/>
@@ -33251,11 +33919,11 @@
       </c>
       <c r="AT7" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.7989999999999999</v>
       </c>
       <c r="AU7" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.7989999999999999</v>
       </c>
       <c r="AV7" s="24" t="e">
         <f t="shared" si="3"/>
@@ -33279,23 +33947,23 @@
       </c>
       <c r="C8" s="21" cm="1">
         <f t="array" ref="C8">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="19" cm="1">
         <f t="array" ref="D8">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="E8" s="19" cm="1">
         <f t="array" ref="E8">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="19" t="e" cm="1">
+        <v>2.4</v>
+      </c>
+      <c r="F8" s="19" cm="1">
         <f t="array" ref="F8">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G8" s="19" t="e" cm="1">
+        <v>2.4</v>
+      </c>
+      <c r="G8" s="19" cm="1">
         <f t="array" ref="G8">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>2.4</v>
       </c>
       <c r="H8" s="22" t="e" cm="1">
         <f t="array" ref="H8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33303,23 +33971,23 @@
       </c>
       <c r="I8" s="19" cm="1">
         <f t="array" ref="I8">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="19" cm="1">
         <f t="array" ref="J8">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>4.8840000000000003</v>
       </c>
       <c r="K8" s="19" cm="1">
         <f t="array" ref="K8">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="19" t="e" cm="1">
+        <v>4.8840000000000003</v>
+      </c>
+      <c r="L8" s="19" cm="1">
         <f t="array" ref="L8">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M8" s="19" t="e" cm="1">
+        <v>4.8840000000000003</v>
+      </c>
+      <c r="M8" s="19" cm="1">
         <f t="array" ref="M8">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>4.8840000000000003</v>
       </c>
       <c r="N8" s="22" t="e" cm="1">
         <f t="array" ref="N8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33349,21 +34017,21 @@
         <f t="array" ref="T8">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A8)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B8)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U8" s="29" t="e">
+      <c r="U8" s="29">
         <f t="shared" ref="U8" si="11">J8/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V8" s="3" t="e">
+        <v>2.0350000000000001</v>
+      </c>
+      <c r="V8" s="3">
         <f t="shared" ref="V8" si="12">K8/E8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="3" t="e">
+        <v>2.0350000000000001</v>
+      </c>
+      <c r="W8" s="3">
         <f t="shared" ref="W8" si="13">L8/F8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X8" s="3" t="e">
+        <v>2.0350000000000001</v>
+      </c>
+      <c r="X8" s="3">
         <f t="shared" ref="X8" si="14">M8/G8</f>
-        <v>#NUM!</v>
+        <v>2.0350000000000001</v>
       </c>
       <c r="Y8" s="4" t="e">
         <f t="shared" ref="Y8" si="15">N8/H8</f>
@@ -33371,31 +34039,31 @@
       </c>
       <c r="Z8" s="26">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2.4840000000000004</v>
       </c>
       <c r="AA8" s="24">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="AB8" s="24" t="e">
+        <v>2.4840000000000004</v>
+      </c>
+      <c r="AB8" s="24">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC8" s="24" t="e">
+        <v>2.4840000000000004</v>
+      </c>
+      <c r="AC8" s="24">
         <f t="shared" si="9"/>
-        <v>#NUM!</v>
+        <v>2.4840000000000004</v>
       </c>
       <c r="AD8" s="27" t="e">
         <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE8" s="26" t="e">
+      <c r="AE8" s="26">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF8" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="24">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG8" s="24" t="e">
         <f t="shared" si="0"/>
@@ -33411,11 +34079,11 @@
       </c>
       <c r="AJ8" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.4</v>
       </c>
       <c r="AK8" s="24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2.4</v>
       </c>
       <c r="AL8" s="24" t="e">
         <f t="shared" si="1"/>
@@ -33451,11 +34119,11 @@
       </c>
       <c r="AT8" s="26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.8840000000000003</v>
       </c>
       <c r="AU8" s="24">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.8840000000000003</v>
       </c>
       <c r="AV8" s="24" t="e">
         <f t="shared" si="3"/>
@@ -33479,23 +34147,23 @@
       </c>
       <c r="C9" s="21" cm="1">
         <f t="array" ref="C9">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="19" cm="1">
         <f t="array" ref="D9">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.6360000000000001</v>
       </c>
       <c r="E9" s="19" cm="1">
         <f t="array" ref="E9">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="19" t="e" cm="1">
+        <v>5.6360000000000001</v>
+      </c>
+      <c r="F9" s="19" cm="1">
         <f t="array" ref="F9">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G9" s="19" t="e" cm="1">
+        <v>5.6360000000000001</v>
+      </c>
+      <c r="G9" s="19" cm="1">
         <f t="array" ref="G9">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.6360000000000001</v>
       </c>
       <c r="H9" s="22" t="e" cm="1">
         <f t="array" ref="H9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33503,23 +34171,23 @@
       </c>
       <c r="I9" s="19" cm="1">
         <f t="array" ref="I9">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="19" cm="1">
         <f t="array" ref="J9">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>6.8319999999999999</v>
       </c>
       <c r="K9" s="19" cm="1">
         <f t="array" ref="K9">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="19" t="e" cm="1">
+        <v>6.8319999999999999</v>
+      </c>
+      <c r="L9" s="19" cm="1">
         <f t="array" ref="L9">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="19" t="e" cm="1">
+        <v>6.8319999999999999</v>
+      </c>
+      <c r="M9" s="19" cm="1">
         <f t="array" ref="M9">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>6.8319999999999999</v>
       </c>
       <c r="N9" s="22" t="e" cm="1">
         <f t="array" ref="N9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33549,21 +34217,21 @@
         <f t="array" ref="T9">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A9)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B9)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U9" s="3" t="e">
+      <c r="U9" s="3">
         <f t="shared" ref="U9:U12" si="16">J9/D9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V9" s="3" t="e">
+        <v>1.2122072391767211</v>
+      </c>
+      <c r="V9" s="3">
         <f t="shared" ref="V9:V12" si="17">K9/E9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W9" s="3" t="e">
+        <v>1.2122072391767211</v>
+      </c>
+      <c r="W9" s="3">
         <f t="shared" ref="W9:W12" si="18">L9/F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X9" s="3" t="e">
+        <v>1.2122072391767211</v>
+      </c>
+      <c r="X9" s="3">
         <f t="shared" ref="X9:X12" si="19">M9/G9</f>
-        <v>#NUM!</v>
+        <v>1.2122072391767211</v>
       </c>
       <c r="Y9" s="4" t="e">
         <f t="shared" ref="Y9:Y12" si="20">N9/H9</f>
@@ -33571,31 +34239,31 @@
       </c>
       <c r="Z9" s="24">
         <f t="shared" ref="Z9:Z12" si="21">J9-D9</f>
-        <v>0</v>
+        <v>1.1959999999999997</v>
       </c>
       <c r="AA9" s="24">
         <f t="shared" ref="AA9:AA12" si="22">K9-E9</f>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="24" t="e">
+        <v>1.1959999999999997</v>
+      </c>
+      <c r="AB9" s="24">
         <f t="shared" ref="AB9:AB12" si="23">L9-F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC9" s="24" t="e">
+        <v>1.1959999999999997</v>
+      </c>
+      <c r="AC9" s="24">
         <f t="shared" ref="AC9:AC12" si="24">M9-G9</f>
-        <v>#NUM!</v>
+        <v>1.1959999999999997</v>
       </c>
       <c r="AD9" s="27" t="e">
         <f t="shared" ref="AD9:AD12" si="25">N9-H9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE9" s="24" t="e">
+      <c r="AE9" s="24">
         <f t="shared" ref="AE9:AE12" si="26">P9/D9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF9" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="24">
         <f t="shared" ref="AF9:AF12" si="27">Q9/E9</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG9" s="24" t="e">
         <f t="shared" ref="AG9:AG12" si="28">R9/F9</f>
@@ -33611,11 +34279,11 @@
       </c>
       <c r="AJ9" s="24">
         <f t="shared" ref="AJ9:AJ12" si="31">P9-D9</f>
-        <v>0</v>
+        <v>-5.6360000000000001</v>
       </c>
       <c r="AK9" s="24">
         <f t="shared" ref="AK9:AK12" si="32">Q9-E9</f>
-        <v>0</v>
+        <v>-5.6360000000000001</v>
       </c>
       <c r="AL9" s="24" t="e">
         <f t="shared" ref="AL9:AL12" si="33">R9-F9</f>
@@ -33651,11 +34319,11 @@
       </c>
       <c r="AT9" s="24">
         <f t="shared" ref="AT9:AT12" si="41">J9 - P9</f>
-        <v>0</v>
+        <v>6.8319999999999999</v>
       </c>
       <c r="AU9" s="24">
         <f t="shared" ref="AU9:AU12" si="42">K9 - Q9</f>
-        <v>0</v>
+        <v>6.8319999999999999</v>
       </c>
       <c r="AV9" s="24" t="e">
         <f t="shared" ref="AV9:AV12" si="43">L9 - R9</f>
@@ -33679,23 +34347,23 @@
       </c>
       <c r="C10" s="21" cm="1">
         <f t="array" ref="C10">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="19" cm="1">
         <f t="array" ref="D10">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>2.532</v>
       </c>
       <c r="E10" s="19" cm="1">
         <f t="array" ref="E10">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="19" t="e" cm="1">
+        <v>2.532</v>
+      </c>
+      <c r="F10" s="19" cm="1">
         <f t="array" ref="F10">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G10" s="19" t="e" cm="1">
+        <v>2.532</v>
+      </c>
+      <c r="G10" s="19" cm="1">
         <f t="array" ref="G10">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>2.532</v>
       </c>
       <c r="H10" s="22" t="e" cm="1">
         <f t="array" ref="H10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33703,23 +34371,23 @@
       </c>
       <c r="I10" s="19" cm="1">
         <f t="array" ref="I10">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="19" cm="1">
         <f t="array" ref="J10">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>3.1619999999999999</v>
       </c>
       <c r="K10" s="19" cm="1">
         <f t="array" ref="K10">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L10" s="19" t="e" cm="1">
+        <v>3.1619999999999999</v>
+      </c>
+      <c r="L10" s="19" cm="1">
         <f t="array" ref="L10">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="19" t="e" cm="1">
+        <v>3.1619999999999999</v>
+      </c>
+      <c r="M10" s="19" cm="1">
         <f t="array" ref="M10">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>3.1619999999999999</v>
       </c>
       <c r="N10" s="22" t="e" cm="1">
         <f t="array" ref="N10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33749,21 +34417,21 @@
         <f t="array" ref="T10">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A10)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B10)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U10" s="3" t="e">
+      <c r="U10" s="3">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V10" s="3" t="e">
+        <v>1.2488151658767772</v>
+      </c>
+      <c r="V10" s="3">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W10" s="3" t="e">
+        <v>1.2488151658767772</v>
+      </c>
+      <c r="W10" s="3">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X10" s="3" t="e">
+        <v>1.2488151658767772</v>
+      </c>
+      <c r="X10" s="3">
         <f t="shared" si="19"/>
-        <v>#NUM!</v>
+        <v>1.2488151658767772</v>
       </c>
       <c r="Y10" s="4" t="e">
         <f t="shared" si="20"/>
@@ -33771,31 +34439,31 @@
       </c>
       <c r="Z10" s="24">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>0.62999999999999989</v>
       </c>
       <c r="AA10" s="24">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="24" t="e">
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="AB10" s="24">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC10" s="24" t="e">
+        <v>0.62999999999999989</v>
+      </c>
+      <c r="AC10" s="24">
         <f t="shared" si="24"/>
-        <v>#NUM!</v>
+        <v>0.62999999999999989</v>
       </c>
       <c r="AD10" s="27" t="e">
         <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE10" s="24" t="e">
+      <c r="AE10" s="24">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF10" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="24">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="24" t="e">
         <f t="shared" si="28"/>
@@ -33811,11 +34479,11 @@
       </c>
       <c r="AJ10" s="24">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>-2.532</v>
       </c>
       <c r="AK10" s="24">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-2.532</v>
       </c>
       <c r="AL10" s="24" t="e">
         <f t="shared" si="33"/>
@@ -33851,11 +34519,11 @@
       </c>
       <c r="AT10" s="24">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>3.1619999999999999</v>
       </c>
       <c r="AU10" s="24">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>3.1619999999999999</v>
       </c>
       <c r="AV10" s="24" t="e">
         <f t="shared" si="43"/>
@@ -33879,23 +34547,23 @@
       </c>
       <c r="C11" s="21" cm="1">
         <f t="array" ref="C11">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="19" cm="1">
         <f t="array" ref="D11">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.4189999999999996</v>
       </c>
       <c r="E11" s="19" cm="1">
         <f t="array" ref="E11">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="19" t="e" cm="1">
+        <v>5.4189999999999996</v>
+      </c>
+      <c r="F11" s="19" cm="1">
         <f t="array" ref="F11">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11" s="19" t="e" cm="1">
+        <v>5.4189999999999996</v>
+      </c>
+      <c r="G11" s="19" cm="1">
         <f t="array" ref="G11">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.4189999999999996</v>
       </c>
       <c r="H11" s="22" t="e" cm="1">
         <f t="array" ref="H11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33903,23 +34571,23 @@
       </c>
       <c r="I11" s="19" cm="1">
         <f t="array" ref="I11">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="19" cm="1">
         <f t="array" ref="J11">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.2069999999999999</v>
       </c>
       <c r="K11" s="19" cm="1">
         <f t="array" ref="K11">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="19" t="e" cm="1">
+        <v>5.2069999999999999</v>
+      </c>
+      <c r="L11" s="19" cm="1">
         <f t="array" ref="L11">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="19" t="e" cm="1">
+        <v>5.2069999999999999</v>
+      </c>
+      <c r="M11" s="19" cm="1">
         <f t="array" ref="M11">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.2069999999999999</v>
       </c>
       <c r="N11" s="22" t="e" cm="1">
         <f t="array" ref="N11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -33949,21 +34617,21 @@
         <f t="array" ref="T11">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A11)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B11)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U11" s="3" t="e">
+      <c r="U11" s="3">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V11" s="3" t="e">
+        <v>0.96087839084701976</v>
+      </c>
+      <c r="V11" s="3">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W11" s="3" t="e">
+        <v>0.96087839084701976</v>
+      </c>
+      <c r="W11" s="3">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X11" s="3" t="e">
+        <v>0.96087839084701976</v>
+      </c>
+      <c r="X11" s="3">
         <f t="shared" si="19"/>
-        <v>#NUM!</v>
+        <v>0.96087839084701976</v>
       </c>
       <c r="Y11" s="4" t="e">
         <f t="shared" si="20"/>
@@ -33971,31 +34639,31 @@
       </c>
       <c r="Z11" s="24">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>-0.21199999999999974</v>
       </c>
       <c r="AA11" s="24">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="AB11" s="24" t="e">
+        <v>-0.21199999999999974</v>
+      </c>
+      <c r="AB11" s="24">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC11" s="24" t="e">
+        <v>-0.21199999999999974</v>
+      </c>
+      <c r="AC11" s="24">
         <f t="shared" si="24"/>
-        <v>#NUM!</v>
+        <v>-0.21199999999999974</v>
       </c>
       <c r="AD11" s="27" t="e">
         <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE11" s="24" t="e">
+      <c r="AE11" s="24">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF11" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="24">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG11" s="24" t="e">
         <f t="shared" si="28"/>
@@ -34011,11 +34679,11 @@
       </c>
       <c r="AJ11" s="24">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>-5.4189999999999996</v>
       </c>
       <c r="AK11" s="24">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-5.4189999999999996</v>
       </c>
       <c r="AL11" s="24" t="e">
         <f t="shared" si="33"/>
@@ -34051,11 +34719,11 @@
       </c>
       <c r="AT11" s="24">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>5.2069999999999999</v>
       </c>
       <c r="AU11" s="24">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>5.2069999999999999</v>
       </c>
       <c r="AV11" s="24" t="e">
         <f t="shared" si="43"/>
@@ -34079,23 +34747,23 @@
       </c>
       <c r="C12" s="21" cm="1">
         <f t="array" ref="C12">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="19" cm="1">
         <f t="array" ref="D12">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="E12" s="19" cm="1">
         <f t="array" ref="E12">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="19" t="e" cm="1">
+        <v>4.5259999999999998</v>
+      </c>
+      <c r="F12" s="19" cm="1">
         <f t="array" ref="F12">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" s="19" t="e" cm="1">
+        <v>4.5259999999999998</v>
+      </c>
+      <c r="G12" s="19" cm="1">
         <f t="array" ref="G12">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="H12" s="22" t="e" cm="1">
         <f t="array" ref="H12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Local"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -34103,23 +34771,23 @@
       </c>
       <c r="I12" s="19" cm="1">
         <f t="array" ref="I12">COUNT(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="19" cm="1">
         <f t="array" ref="J12">MIN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
+        <v>5.5060000000000002</v>
       </c>
       <c r="K12" s="19" cm="1">
         <f t="array" ref="K12">MAX(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="19" t="e" cm="1">
+        <v>5.5060000000000002</v>
+      </c>
+      <c r="L12" s="19" cm="1">
         <f t="array" ref="L12">AVERAGE(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="19" t="e" cm="1">
+        <v>5.5060000000000002</v>
+      </c>
+      <c r="M12" s="19" cm="1">
         <f t="array" ref="M12">MEDIAN(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
-        <v>#NUM!</v>
+        <v>5.5060000000000002</v>
       </c>
       <c r="N12" s="22" t="e" cm="1">
         <f t="array" ref="N12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Local")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
@@ -34149,21 +34817,21 @@
         <f t="array" ref="T12">STDEV(IF(('ibbs-web-app-metrics'!$F$2:$F$9999=$A12)*('ibbs-web-app-metrics'!$G$2:$G$9999=$B12)*('ibbs-web-app-metrics'!$B$2:$B$9999="Remote")*('ibbs-web-app-metrics'!$C$2:$C$9999="Remote"), 'ibbs-web-app-metrics'!$J$2:$J$9999))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U12" s="3" t="e">
+      <c r="U12" s="3">
         <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V12" s="3" t="e">
+        <v>1.2165267344233319</v>
+      </c>
+      <c r="V12" s="3">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W12" s="3" t="e">
+        <v>1.2165267344233319</v>
+      </c>
+      <c r="W12" s="3">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X12" s="3" t="e">
+        <v>1.2165267344233319</v>
+      </c>
+      <c r="X12" s="3">
         <f t="shared" si="19"/>
-        <v>#NUM!</v>
+        <v>1.2165267344233319</v>
       </c>
       <c r="Y12" s="4" t="e">
         <f t="shared" si="20"/>
@@ -34171,31 +34839,31 @@
       </c>
       <c r="Z12" s="24">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>0.98000000000000043</v>
       </c>
       <c r="AA12" s="24">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="AB12" s="24" t="e">
+        <v>0.98000000000000043</v>
+      </c>
+      <c r="AB12" s="24">
         <f t="shared" si="23"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AC12" s="24" t="e">
+        <v>0.98000000000000043</v>
+      </c>
+      <c r="AC12" s="24">
         <f t="shared" si="24"/>
-        <v>#NUM!</v>
+        <v>0.98000000000000043</v>
       </c>
       <c r="AD12" s="27" t="e">
         <f t="shared" si="25"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE12" s="24" t="e">
+      <c r="AE12" s="24">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF12" s="24" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="24">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AG12" s="24" t="e">
         <f t="shared" si="28"/>
@@ -34211,11 +34879,11 @@
       </c>
       <c r="AJ12" s="24">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>-4.5259999999999998</v>
       </c>
       <c r="AK12" s="24">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>-4.5259999999999998</v>
       </c>
       <c r="AL12" s="24" t="e">
         <f t="shared" si="33"/>
@@ -34251,11 +34919,11 @@
       </c>
       <c r="AT12" s="24">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>5.5060000000000002</v>
       </c>
       <c r="AU12" s="24">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>5.5060000000000002</v>
       </c>
       <c r="AV12" s="24" t="e">
         <f t="shared" si="43"/>

</xml_diff>

<commit_message>
added documentation for the summary worksheet
</commit_message>
<xml_diff>
--- a/performance metrics/ibbs-web-app-metrics-combined.xlsx
+++ b/performance metrics/ibbs-web-app-metrics-combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse.abdul\Documents\Version Control\Git\ibbs-web-app-metrics\performance metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1031E9EB-D808-42C8-A30E-D2DF4B0AF7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB8EAB22-23E3-4192-AD45-C716868A339A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2595" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2595" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ibbs-web-app-metrics" sheetId="1" r:id="rId1"/>
@@ -1886,12 +1886,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1899,6 +1893,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2258,9 +2258,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L9999"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L31"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2269,7 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="9" customWidth="1"/>
     <col min="6" max="7" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="8"/>
     <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -2311,7 +2311,7 @@
       <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -42941,7 +42941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AX64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -42957,30 +42957,30 @@
     <row r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="35" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="37"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="35"/>
       <c r="U1" s="30" t="s">
         <v>32</v>
       </c>
@@ -45177,14 +45177,14 @@
       </c>
     </row>
     <row r="14" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
       <c r="U14" s="30" t="s">
         <v>42</v>
       </c>
@@ -46865,14 +46865,14 @@
       </c>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
       <c r="I27" s="30" t="s">
         <v>48</v>
       </c>
@@ -48997,14 +48997,14 @@
       </c>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="37"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="35"/>
       <c r="U40" s="30" t="s">
         <v>55</v>
       </c>
@@ -50685,14 +50685,14 @@
       </c>
     </row>
     <row r="53" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="37"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="35"/>
       <c r="U53" s="30" t="s">
         <v>61</v>
       </c>
@@ -52374,18 +52374,19 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="AT40:AX40"/>
-    <mergeCell ref="U53:Y53"/>
-    <mergeCell ref="Z53:AD53"/>
-    <mergeCell ref="AE53:AI53"/>
-    <mergeCell ref="AJ53:AN53"/>
-    <mergeCell ref="AO53:AS53"/>
-    <mergeCell ref="AT53:AX53"/>
-    <mergeCell ref="U40:Y40"/>
-    <mergeCell ref="Z40:AD40"/>
-    <mergeCell ref="AE40:AI40"/>
-    <mergeCell ref="AJ40:AN40"/>
-    <mergeCell ref="AO40:AS40"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:T1"/>
+    <mergeCell ref="AE1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="AO1:AS1"/>
     <mergeCell ref="AT14:AX14"/>
     <mergeCell ref="I27:M27"/>
     <mergeCell ref="O27:S27"/>
@@ -52400,19 +52401,18 @@
     <mergeCell ref="AE14:AI14"/>
     <mergeCell ref="AJ14:AN14"/>
     <mergeCell ref="AO14:AS14"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="AO1:AS1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:T1"/>
-    <mergeCell ref="AE1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AT40:AX40"/>
+    <mergeCell ref="U53:Y53"/>
+    <mergeCell ref="Z53:AD53"/>
+    <mergeCell ref="AE53:AI53"/>
+    <mergeCell ref="AJ53:AN53"/>
+    <mergeCell ref="AO53:AS53"/>
+    <mergeCell ref="AT53:AX53"/>
+    <mergeCell ref="U40:Y40"/>
+    <mergeCell ref="Z40:AD40"/>
+    <mergeCell ref="AE40:AI40"/>
+    <mergeCell ref="AJ40:AN40"/>
+    <mergeCell ref="AO40:AS40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>